<commit_message>
Weekend-Weekday model  validation over different months
</commit_message>
<xml_diff>
--- a/August 2018/Weekend-Weekday/Validation/Input_August2018.xlsx
+++ b/August 2018/Weekend-Weekday/Validation/Input_August2018.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C172115-13F8-4A87-938D-E48697FA8152}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FA3A31-5598-4096-9C31-C092DD54D4EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inflow" sheetId="4" r:id="rId1"/>
@@ -799,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE87C648-8DC5-4696-853D-D597AF6BA2AD}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -817,248 +817,248 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17">
-        <v>1658</v>
+      <c r="B2" s="18">
+        <v>3830</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="17">
-        <v>1655</v>
+      <c r="B3" s="18">
+        <v>2818</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="17">
-        <v>1652</v>
+      <c r="B4" s="18">
+        <v>3918</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="17">
-        <v>1650</v>
+      <c r="B5" s="18">
+        <v>4446</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="17">
-        <v>1648</v>
+      <c r="B6" s="18">
+        <v>2018</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="17">
-        <v>1646</v>
+      <c r="B7" s="18">
+        <v>6232</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="17">
-        <v>1643</v>
+      <c r="B8" s="18">
+        <v>3466</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="17">
-        <v>1640</v>
+      <c r="B9" s="18">
+        <v>3338</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="17">
-        <v>1637</v>
+      <c r="B10" s="18">
+        <v>3391</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="17">
-        <v>1634</v>
+      <c r="B11" s="18">
+        <v>4572</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="17">
-        <v>1632</v>
+      <c r="B12" s="18">
+        <v>1374</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="17">
-        <v>1630</v>
+      <c r="B13" s="18">
+        <v>2797</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="17">
-        <v>1627</v>
+      <c r="B14" s="18">
+        <v>1959</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="17">
-        <v>1625</v>
+      <c r="B15" s="18">
+        <v>6463</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="17">
-        <v>1621</v>
+      <c r="B16" s="18">
+        <v>3023</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="17">
-        <v>1618</v>
+      <c r="B17" s="18">
+        <v>2551</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="17">
-        <v>1615</v>
+      <c r="B18" s="18">
+        <v>2535</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="17">
-        <v>1614</v>
+      <c r="B19" s="18">
+        <v>5622</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="17">
-        <v>1612</v>
+      <c r="B20" s="18">
+        <v>3503</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="17">
-        <v>1609</v>
+      <c r="B21" s="18">
+        <v>2680</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="17">
-        <v>1607</v>
+      <c r="B22" s="18">
+        <v>6297</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="17">
-        <v>1605</v>
+      <c r="B23" s="18">
+        <v>6402</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="17">
-        <v>1603</v>
+      <c r="B24" s="18">
+        <v>5466</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="17">
-        <v>1601</v>
+      <c r="B25" s="18">
+        <v>7411</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="17">
-        <v>1599</v>
+      <c r="B26" s="18">
+        <v>2189</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="17">
-        <v>1597</v>
+      <c r="B27" s="18">
+        <v>2186</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="17">
-        <v>1595</v>
+      <c r="B28" s="18">
+        <v>6602</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="17">
-        <v>1592</v>
+      <c r="B29" s="18">
+        <v>5950</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="17">
-        <v>1590</v>
+      <c r="B30" s="18">
+        <v>5347</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="17">
-        <v>1588</v>
+      <c r="B31" s="18">
+        <v>4347</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="17">
-        <v>1586</v>
+      <c r="B32" s="18">
+        <v>8417</v>
       </c>
     </row>
   </sheetData>
@@ -1360,7 +1360,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1378,248 +1378,248 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17">
-        <v>3603.56</v>
+      <c r="B2" s="18">
+        <v>1658</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="17">
-        <v>3603.3</v>
+      <c r="B3" s="18">
+        <v>1655</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="17">
-        <v>3603.06</v>
+      <c r="B4" s="18">
+        <v>1652</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="17">
-        <v>3602.91</v>
+      <c r="B5" s="18">
+        <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="17">
-        <v>3602.72</v>
+      <c r="B6" s="18">
+        <v>1648</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="17">
-        <v>3602.52</v>
+      <c r="B7" s="18">
+        <v>1646</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="17">
-        <v>3602.27</v>
+      <c r="B8" s="18">
+        <v>1643</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="17">
-        <v>3602.02</v>
+      <c r="B9" s="18">
+        <v>1640</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="17">
-        <v>3601.77</v>
+      <c r="B10" s="18">
+        <v>1637</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="17">
-        <v>3601.54</v>
+      <c r="B11" s="18">
+        <v>1634</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="17">
-        <v>3601.33</v>
+      <c r="B12" s="18">
+        <v>1632</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="17">
-        <v>3601.18</v>
+      <c r="B13" s="18">
+        <v>1630</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="17">
-        <v>3600.9</v>
+      <c r="B14" s="18">
+        <v>1627</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="17">
-        <v>3600.71</v>
+      <c r="B15" s="18">
+        <v>1625</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="17">
-        <v>3600.45</v>
+      <c r="B16" s="18">
+        <v>1621</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="17">
-        <v>3600.18</v>
+      <c r="B17" s="18">
+        <v>1618</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="17">
-        <v>3599.91</v>
+      <c r="B18" s="18">
+        <v>1615</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="17">
-        <v>3599.78</v>
+      <c r="B19" s="18">
+        <v>1614</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="17">
-        <v>3599.61</v>
+      <c r="B20" s="18">
+        <v>1612</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="17">
-        <v>3599.34</v>
+      <c r="B21" s="18">
+        <v>1609</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="17">
-        <v>3599.14</v>
+      <c r="B22" s="18">
+        <v>1607</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="17">
-        <v>3598.94</v>
+      <c r="B23" s="18">
+        <v>1605</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="17">
-        <v>3598.72</v>
+      <c r="B24" s="18">
+        <v>1603</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="17">
-        <v>3598.54</v>
+      <c r="B25" s="18">
+        <v>1601</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="17">
-        <v>3598.34</v>
+      <c r="B26" s="18">
+        <v>1599</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="17">
-        <v>3598.15</v>
+      <c r="B27" s="18">
+        <v>1597</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="17">
-        <v>3597.95</v>
+      <c r="B28" s="18">
+        <v>1595</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="17">
-        <v>3597.74</v>
+      <c r="B29" s="18">
+        <v>1592</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="17">
-        <v>3597.52</v>
+      <c r="B30" s="18">
+        <v>1590</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="17">
-        <v>3597.28</v>
+      <c r="B31" s="18">
+        <v>1588</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="17">
-        <v>3597.12</v>
+      <c r="B32" s="18">
+        <v>1586</v>
       </c>
     </row>
   </sheetData>
@@ -1631,7 +1631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B28808B-0EB8-47F9-9AD0-E6038F040C69}">
   <dimension ref="A1:O2977"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
@@ -1642,7 +1642,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>59</v>
       </c>
       <c r="B1" t="s">

</xml_diff>